<commit_message>
Successfully organized project directory, also fixed bug in studentDropdown
</commit_message>
<xml_diff>
--- a/data/3201.xlsx
+++ b/data/3201.xlsx
@@ -3547,37 +3547,37 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>9.4</v>
+        <v>4.4</v>
       </c>
       <c r="C2" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="D2" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="D2" t="n">
-        <v>6.5</v>
-      </c>
       <c r="E2" t="n">
-        <v>6.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="G2" t="n">
-        <v>9.699999999999999</v>
+        <v>8.6</v>
       </c>
       <c r="H2" t="n">
-        <v>2.8</v>
+        <v>3</v>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>5.2</v>
       </c>
       <c r="J2" t="n">
-        <v>9.6</v>
+        <v>10</v>
       </c>
       <c r="K2" t="n">
-        <v>7.6</v>
+        <v>6</v>
       </c>
       <c r="L2" t="n">
-        <v>7</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="3">
@@ -3587,37 +3587,37 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>10</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C3" t="n">
-        <v>9.9</v>
+        <v>3.7</v>
       </c>
       <c r="D3" t="n">
-        <v>8.6</v>
+        <v>3.4</v>
       </c>
       <c r="E3" t="n">
-        <v>5.6</v>
+        <v>7.5</v>
       </c>
       <c r="F3" t="n">
-        <v>7</v>
+        <v>1.6</v>
       </c>
       <c r="G3" t="n">
-        <v>4.8</v>
+        <v>7.4</v>
       </c>
       <c r="H3" t="n">
-        <v>8.699999999999999</v>
+        <v>4.7</v>
       </c>
       <c r="I3" t="n">
-        <v>2.6</v>
+        <v>1.6</v>
       </c>
       <c r="J3" t="n">
-        <v>2.4</v>
+        <v>9.4</v>
       </c>
       <c r="K3" t="n">
-        <v>4.8</v>
+        <v>3.2</v>
       </c>
       <c r="L3" t="n">
-        <v>3.9</v>
+        <v>2.1</v>
       </c>
     </row>
     <row r="4">
@@ -3627,37 +3627,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>6.2</v>
+        <v>3.6</v>
       </c>
       <c r="C4" t="n">
-        <v>6</v>
+        <v>8.9</v>
       </c>
       <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
         <v>6.4</v>
       </c>
-      <c r="E4" t="n">
-        <v>7.1</v>
-      </c>
       <c r="F4" t="n">
-        <v>6.9</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="G4" t="n">
-        <v>8.1</v>
+        <v>5.9</v>
       </c>
       <c r="H4" t="n">
-        <v>8.6</v>
+        <v>7.2</v>
       </c>
       <c r="I4" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="J4" t="n">
-        <v>8.199999999999999</v>
+        <v>4.9</v>
       </c>
       <c r="K4" t="n">
-        <v>3.7</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="L4" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="5">
@@ -3670,34 +3670,34 @@
         <v>7.4</v>
       </c>
       <c r="C5" t="n">
-        <v>8.699999999999999</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="D5" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E5" t="n">
         <v>8.6</v>
       </c>
       <c r="F5" t="n">
-        <v>3.8</v>
+        <v>7.2</v>
       </c>
       <c r="G5" t="n">
-        <v>7.4</v>
+        <v>6.6</v>
       </c>
       <c r="H5" t="n">
-        <v>3.6</v>
+        <v>2.6</v>
       </c>
       <c r="I5" t="n">
-        <v>4.2</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="J5" t="n">
-        <v>5.4</v>
+        <v>5.6</v>
       </c>
       <c r="K5" t="n">
-        <v>5</v>
+        <v>7.3</v>
       </c>
       <c r="L5" t="n">
-        <v>8.4</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="6">
@@ -3707,37 +3707,37 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.1</v>
+        <v>7.3</v>
       </c>
       <c r="C6" t="n">
-        <v>9.9</v>
+        <v>5.9</v>
       </c>
       <c r="D6" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E6" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2.7</v>
+      </c>
+      <c r="G6" t="n">
+        <v>2.8</v>
+      </c>
+      <c r="H6" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="I6" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="J6" t="n">
         <v>7.2</v>
       </c>
-      <c r="E6" t="n">
-        <v>5.3</v>
-      </c>
-      <c r="F6" t="n">
-        <v>6.7</v>
-      </c>
-      <c r="G6" t="n">
-        <v>8.800000000000001</v>
-      </c>
-      <c r="H6" t="n">
-        <v>4</v>
-      </c>
-      <c r="I6" t="n">
-        <v>7.6</v>
-      </c>
-      <c r="J6" t="n">
-        <v>5.2</v>
-      </c>
       <c r="K6" t="n">
-        <v>7</v>
+        <v>7.8</v>
       </c>
       <c r="L6" t="n">
-        <v>9</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="7">
@@ -3747,37 +3747,37 @@
         </is>
       </c>
       <c r="B7" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="C7" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9.1</v>
+      </c>
+      <c r="E7" t="n">
         <v>7.6</v>
       </c>
-      <c r="C7" t="n">
-        <v>7.2</v>
-      </c>
-      <c r="D7" t="n">
-        <v>4.6</v>
-      </c>
-      <c r="E7" t="n">
-        <v>8.6</v>
-      </c>
       <c r="F7" t="n">
-        <v>6.4</v>
+        <v>7.8</v>
       </c>
       <c r="G7" t="n">
-        <v>4.1</v>
+        <v>9.9</v>
       </c>
       <c r="H7" t="n">
-        <v>3.4</v>
+        <v>2.8</v>
       </c>
       <c r="I7" t="n">
-        <v>8.199999999999999</v>
+        <v>5.9</v>
       </c>
       <c r="J7" t="n">
-        <v>8.199999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="K7" t="n">
-        <v>4.9</v>
+        <v>6.6</v>
       </c>
       <c r="L7" t="n">
-        <v>7</v>
+        <v>7.4</v>
       </c>
     </row>
     <row r="8">
@@ -3787,37 +3787,37 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>7.8</v>
       </c>
       <c r="C8" t="n">
-        <v>5.1</v>
+        <v>6.9</v>
       </c>
       <c r="D8" t="n">
-        <v>3.7</v>
+        <v>4.4</v>
       </c>
       <c r="E8" t="n">
-        <v>9.4</v>
+        <v>6</v>
       </c>
       <c r="F8" t="n">
-        <v>4.6</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G8" t="n">
-        <v>8.6</v>
+        <v>7.6</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7</v>
+        <v>4</v>
       </c>
       <c r="I8" t="n">
-        <v>9.4</v>
+        <v>6.6</v>
       </c>
       <c r="J8" t="n">
-        <v>8.9</v>
+        <v>3.8</v>
       </c>
       <c r="K8" t="n">
-        <v>6.4</v>
+        <v>9.6</v>
       </c>
       <c r="L8" t="n">
-        <v>8.800000000000001</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="9">
@@ -3827,37 +3827,37 @@
         </is>
       </c>
       <c r="B9" t="n">
+        <v>9.6</v>
+      </c>
+      <c r="C9" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="D9" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="E9" t="n">
+        <v>9.199999999999999</v>
+      </c>
+      <c r="F9" t="n">
         <v>4.6</v>
       </c>
-      <c r="C9" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="D9" t="n">
-        <v>4.1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>6.9</v>
-      </c>
-      <c r="F9" t="n">
-        <v>9.4</v>
-      </c>
       <c r="G9" t="n">
-        <v>7.8</v>
+        <v>6.7</v>
       </c>
       <c r="H9" t="n">
-        <v>3.3</v>
+        <v>3</v>
       </c>
       <c r="I9" t="n">
-        <v>6.2</v>
+        <v>5.2</v>
       </c>
       <c r="J9" t="n">
-        <v>4.1</v>
+        <v>9</v>
       </c>
       <c r="K9" t="n">
-        <v>3.9</v>
+        <v>6.4</v>
       </c>
       <c r="L9" t="n">
-        <v>7.2</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="10">
@@ -3867,37 +3867,37 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>9.4</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="C10" t="n">
-        <v>8.1</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="D10" t="n">
-        <v>4.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>7.5</v>
+        <v>6.2</v>
       </c>
       <c r="F10" t="n">
-        <v>4</v>
+        <v>7.4</v>
       </c>
       <c r="G10" t="n">
-        <v>9.800000000000001</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="H10" t="n">
-        <v>3.4</v>
+        <v>7.4</v>
       </c>
       <c r="I10" t="n">
-        <v>7.4</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="J10" t="n">
-        <v>6.9</v>
+        <v>6.4</v>
       </c>
       <c r="K10" t="n">
         <v>7</v>
       </c>
       <c r="L10" t="n">
-        <v>7.6</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="11">
@@ -3907,7 +3907,7 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>5.6</v>
       </c>
       <c r="C11" t="n">
         <v>7.8</v>
@@ -3916,28 +3916,28 @@
         <v>7.4</v>
       </c>
       <c r="E11" t="n">
+        <v>7.8</v>
+      </c>
+      <c r="F11" t="n">
+        <v>6.7</v>
+      </c>
+      <c r="G11" t="n">
         <v>6.8</v>
       </c>
-      <c r="F11" t="n">
-        <v>3.3</v>
-      </c>
-      <c r="G11" t="n">
-        <v>10</v>
-      </c>
       <c r="H11" t="n">
-        <v>2.1</v>
+        <v>3.1</v>
       </c>
       <c r="I11" t="n">
-        <v>1.4</v>
+        <v>6.2</v>
       </c>
       <c r="J11" t="n">
-        <v>5.4</v>
+        <v>6.2</v>
       </c>
       <c r="K11" t="n">
-        <v>9.199999999999999</v>
+        <v>6</v>
       </c>
       <c r="L11" t="n">
-        <v>2.1</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="12">
@@ -3947,37 +3947,37 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>6.2</v>
+        <v>5.9</v>
       </c>
       <c r="C12" t="n">
         <v>9.4</v>
       </c>
       <c r="D12" t="n">
-        <v>5.5</v>
+        <v>8.4</v>
       </c>
       <c r="E12" t="n">
-        <v>7.3</v>
+        <v>6.7</v>
       </c>
       <c r="F12" t="n">
-        <v>8.1</v>
+        <v>5.4</v>
       </c>
       <c r="G12" t="n">
-        <v>7.6</v>
+        <v>6.3</v>
       </c>
       <c r="H12" t="n">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="I12" t="n">
-        <v>8.6</v>
+        <v>8</v>
       </c>
       <c r="J12" t="n">
-        <v>6.2</v>
+        <v>7</v>
       </c>
       <c r="K12" t="n">
-        <v>10</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="L12" t="n">
-        <v>7.2</v>
+        <v>3.3</v>
       </c>
     </row>
     <row r="13">
@@ -3987,37 +3987,37 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>9.4</v>
+        <v>7.2</v>
       </c>
       <c r="C13" t="n">
-        <v>9.5</v>
+        <v>9.9</v>
       </c>
       <c r="D13" t="n">
-        <v>8.5</v>
+        <v>4.9</v>
       </c>
       <c r="E13" t="n">
         <v>8.800000000000001</v>
       </c>
       <c r="F13" t="n">
-        <v>4.2</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="G13" t="n">
-        <v>4</v>
+        <v>4.6</v>
       </c>
       <c r="H13" t="n">
-        <v>6</v>
+        <v>7.8</v>
       </c>
       <c r="I13" t="n">
-        <v>9.800000000000001</v>
+        <v>9.4</v>
       </c>
       <c r="J13" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="K13" t="n">
+        <v>9.4</v>
+      </c>
+      <c r="L13" t="n">
         <v>7.4</v>
-      </c>
-      <c r="K13" t="n">
-        <v>8.199999999999999</v>
-      </c>
-      <c r="L13" t="n">
-        <v>4.8</v>
       </c>
     </row>
     <row r="14">
@@ -4027,37 +4027,37 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>5.5</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="C14" t="n">
-        <v>5.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="D14" t="n">
-        <v>7.6</v>
+        <v>4.9</v>
       </c>
       <c r="E14" t="n">
-        <v>5.5</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="F14" t="n">
-        <v>4.2</v>
+        <v>3</v>
       </c>
       <c r="G14" t="n">
-        <v>7.2</v>
+        <v>6.9</v>
       </c>
       <c r="H14" t="n">
-        <v>6.8</v>
+        <v>1.4</v>
       </c>
       <c r="I14" t="n">
-        <v>9.199999999999999</v>
+        <v>7.8</v>
       </c>
       <c r="J14" t="n">
-        <v>5.8</v>
+        <v>4.3</v>
       </c>
       <c r="K14" t="n">
-        <v>8</v>
+        <v>6.2</v>
       </c>
       <c r="L14" t="n">
-        <v>6.5</v>
+        <v>9.800000000000001</v>
       </c>
     </row>
     <row r="15">
@@ -4067,37 +4067,37 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>8.4</v>
+        <v>4.9</v>
       </c>
       <c r="C15" t="n">
-        <v>7.2</v>
+        <v>9.4</v>
       </c>
       <c r="D15" t="n">
-        <v>4.6</v>
+        <v>4.4</v>
       </c>
       <c r="E15" t="n">
-        <v>4.8</v>
+        <v>9.9</v>
       </c>
       <c r="F15" t="n">
-        <v>7.1</v>
+        <v>7.8</v>
       </c>
       <c r="G15" t="n">
-        <v>4.2</v>
+        <v>7.4</v>
       </c>
       <c r="H15" t="n">
-        <v>4.8</v>
+        <v>7.6</v>
       </c>
       <c r="I15" t="n">
-        <v>4.6</v>
+        <v>5.2</v>
       </c>
       <c r="J15" t="n">
-        <v>4.8</v>
+        <v>5</v>
       </c>
       <c r="K15" t="n">
         <v>4.4</v>
       </c>
       <c r="L15" t="n">
-        <v>7.2</v>
+        <v>7.8</v>
       </c>
     </row>
     <row r="16">
@@ -4107,37 +4107,37 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>9</v>
+        <v>3.6</v>
       </c>
       <c r="C16" t="n">
-        <v>6.5</v>
+        <v>5</v>
       </c>
       <c r="D16" t="n">
-        <v>3.4</v>
+        <v>5.6</v>
       </c>
       <c r="E16" t="n">
-        <v>5.5</v>
+        <v>8.4</v>
       </c>
       <c r="F16" t="n">
-        <v>9.199999999999999</v>
+        <v>5.6</v>
       </c>
       <c r="G16" t="n">
-        <v>7.8</v>
+        <v>7.7</v>
       </c>
       <c r="H16" t="n">
-        <v>2.1</v>
+        <v>4.2</v>
       </c>
       <c r="I16" t="n">
-        <v>4.8</v>
+        <v>8.9</v>
       </c>
       <c r="J16" t="n">
-        <v>7.7</v>
+        <v>7.4</v>
       </c>
       <c r="K16" t="n">
-        <v>7</v>
+        <v>6.8</v>
       </c>
       <c r="L16" t="n">
-        <v>9.199999999999999</v>
+        <v>6.1</v>
       </c>
     </row>
     <row r="17">
@@ -4147,37 +4147,37 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>9.199999999999999</v>
+        <v>9</v>
       </c>
       <c r="C17" t="n">
-        <v>8.800000000000001</v>
+        <v>10</v>
       </c>
       <c r="D17" t="n">
-        <v>7.4</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E17" t="n">
-        <v>7.5</v>
+        <v>4.1</v>
       </c>
       <c r="F17" t="n">
-        <v>7.6</v>
+        <v>4.4</v>
       </c>
       <c r="G17" t="n">
         <v>9.1</v>
       </c>
       <c r="H17" t="n">
-        <v>7.8</v>
+        <v>2.2</v>
       </c>
       <c r="I17" t="n">
-        <v>9.800000000000001</v>
+        <v>7</v>
       </c>
       <c r="J17" t="n">
-        <v>5.3</v>
+        <v>9.6</v>
       </c>
       <c r="K17" t="n">
-        <v>3.6</v>
+        <v>8.9</v>
       </c>
       <c r="L17" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
@@ -4187,37 +4187,37 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>6.5</v>
+        <v>8.4</v>
       </c>
       <c r="C18" t="n">
-        <v>9.199999999999999</v>
+        <v>7.7</v>
       </c>
       <c r="D18" t="n">
         <v>7.4</v>
       </c>
       <c r="E18" t="n">
-        <v>7.6</v>
+        <v>9</v>
       </c>
       <c r="F18" t="n">
-        <v>8.199999999999999</v>
+        <v>6.6</v>
       </c>
       <c r="G18" t="n">
-        <v>7.6</v>
+        <v>5.3</v>
       </c>
       <c r="H18" t="n">
-        <v>2.8</v>
+        <v>3.8</v>
       </c>
       <c r="I18" t="n">
         <v>9.800000000000001</v>
       </c>
       <c r="J18" t="n">
-        <v>6.8</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="K18" t="n">
-        <v>8.6</v>
+        <v>7</v>
       </c>
       <c r="L18" t="n">
-        <v>7.8</v>
+        <v>8.4</v>
       </c>
     </row>
     <row r="19">
@@ -4227,37 +4227,37 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="C19" t="n">
-        <v>9</v>
+        <v>5.5</v>
       </c>
       <c r="D19" t="n">
-        <v>7.4</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E19" t="n">
-        <v>5.9</v>
+        <v>7.6</v>
       </c>
       <c r="F19" t="n">
-        <v>5.1</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="G19" t="n">
-        <v>5.6</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="H19" t="n">
-        <v>7.3</v>
+        <v>3.2</v>
       </c>
       <c r="I19" t="n">
-        <v>9.6</v>
+        <v>8.6</v>
       </c>
       <c r="J19" t="n">
-        <v>8.699999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="K19" t="n">
-        <v>5.8</v>
+        <v>7</v>
       </c>
       <c r="L19" t="n">
-        <v>10</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="20">
@@ -4267,37 +4267,37 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5.6</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>8</v>
+        <v>5.1</v>
       </c>
       <c r="D20" t="n">
-        <v>9.6</v>
+        <v>4.3</v>
       </c>
       <c r="E20" t="n">
-        <v>9.4</v>
+        <v>4</v>
       </c>
       <c r="F20" t="n">
-        <v>9.300000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="G20" t="n">
-        <v>6.4</v>
+        <v>4.4</v>
       </c>
       <c r="H20" t="n">
-        <v>0.5</v>
+        <v>4.7</v>
       </c>
       <c r="I20" t="n">
-        <v>8.1</v>
+        <v>8.5</v>
       </c>
       <c r="J20" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="K20" t="n">
         <v>6.6</v>
       </c>
-      <c r="K20" t="n">
-        <v>3.4</v>
-      </c>
       <c r="L20" t="n">
-        <v>7.8</v>
+        <v>7.6</v>
       </c>
     </row>
     <row r="21">
@@ -4307,37 +4307,37 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>9.5</v>
+        <v>7.8</v>
       </c>
       <c r="C21" t="n">
-        <v>9.300000000000001</v>
+        <v>8.5</v>
       </c>
       <c r="D21" t="n">
-        <v>7.6</v>
+        <v>6.4</v>
       </c>
       <c r="E21" t="n">
+        <v>6.4</v>
+      </c>
+      <c r="F21" t="n">
+        <v>9</v>
+      </c>
+      <c r="G21" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="H21" t="n">
+        <v>5</v>
+      </c>
+      <c r="I21" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="J21" t="n">
         <v>4.4</v>
       </c>
-      <c r="F21" t="n">
-        <v>6</v>
-      </c>
-      <c r="G21" t="n">
-        <v>3.5</v>
-      </c>
-      <c r="H21" t="n">
-        <v>7.8</v>
-      </c>
-      <c r="I21" t="n">
-        <v>3.1</v>
-      </c>
-      <c r="J21" t="n">
-        <v>7.4</v>
-      </c>
       <c r="K21" t="n">
-        <v>6.6</v>
+        <v>7.2</v>
       </c>
       <c r="L21" t="n">
-        <v>7.6</v>
+        <v>5.8</v>
       </c>
     </row>
     <row r="22">
@@ -4347,37 +4347,37 @@
         </is>
       </c>
       <c r="B22" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="C22" t="n">
+        <v>6</v>
+      </c>
+      <c r="D22" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="E22" t="n">
         <v>7.8</v>
       </c>
-      <c r="C22" t="n">
+      <c r="F22" t="n">
+        <v>3.9</v>
+      </c>
+      <c r="G22" t="n">
         <v>5.6</v>
       </c>
-      <c r="D22" t="n">
-        <v>6.1</v>
-      </c>
-      <c r="E22" t="n">
-        <v>5.7</v>
-      </c>
-      <c r="F22" t="n">
-        <v>8.6</v>
-      </c>
-      <c r="G22" t="n">
-        <v>8.199999999999999</v>
-      </c>
       <c r="H22" t="n">
-        <v>5.5</v>
+        <v>5.9</v>
       </c>
       <c r="I22" t="n">
-        <v>4.2</v>
+        <v>6.5</v>
       </c>
       <c r="J22" t="n">
-        <v>4.9</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="K22" t="n">
-        <v>5.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="L22" t="n">
-        <v>9.4</v>
+        <v>6.8</v>
       </c>
     </row>
     <row r="23">
@@ -4387,37 +4387,37 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>8.5</v>
+        <v>7.7</v>
       </c>
       <c r="C23" t="n">
-        <v>9.300000000000001</v>
+        <v>5.8</v>
       </c>
       <c r="D23" t="n">
-        <v>7.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="E23" t="n">
-        <v>8.6</v>
+        <v>5.5</v>
       </c>
       <c r="F23" t="n">
-        <v>5.4</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="G23" t="n">
-        <v>8.5</v>
+        <v>8</v>
       </c>
       <c r="H23" t="n">
-        <v>1.8</v>
+        <v>4.2</v>
       </c>
       <c r="I23" t="n">
-        <v>9.4</v>
+        <v>8.300000000000001</v>
       </c>
       <c r="J23" t="n">
-        <v>9.699999999999999</v>
+        <v>7.4</v>
       </c>
       <c r="K23" t="n">
-        <v>8.5</v>
+        <v>9.6</v>
       </c>
       <c r="L23" t="n">
-        <v>9.699999999999999</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="24">
@@ -4427,37 +4427,37 @@
         </is>
       </c>
       <c r="B24" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="C24" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="D24" t="n">
         <v>8.199999999999999</v>
       </c>
-      <c r="C24" t="n">
-        <v>5.8</v>
-      </c>
-      <c r="D24" t="n">
-        <v>5</v>
-      </c>
       <c r="E24" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F24" t="n">
-        <v>6.8</v>
+        <v>1.2</v>
       </c>
       <c r="G24" t="n">
-        <v>9.199999999999999</v>
+        <v>7.2</v>
       </c>
       <c r="H24" t="n">
-        <v>3.7</v>
+        <v>4</v>
       </c>
       <c r="I24" t="n">
-        <v>9.9</v>
+        <v>5.1</v>
       </c>
       <c r="J24" t="n">
-        <v>6.4</v>
+        <v>7.4</v>
       </c>
       <c r="K24" t="n">
-        <v>4.2</v>
+        <v>6.7</v>
       </c>
       <c r="L24" t="n">
-        <v>5.6</v>
+        <v>4.6</v>
       </c>
     </row>
     <row r="25">
@@ -4467,37 +4467,37 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>6.2</v>
+        <v>8.4</v>
       </c>
       <c r="C25" t="n">
-        <v>8.4</v>
+        <v>5.2</v>
       </c>
       <c r="D25" t="n">
-        <v>5.8</v>
+        <v>3.6</v>
       </c>
       <c r="E25" t="n">
-        <v>4.6</v>
+        <v>4.4</v>
       </c>
       <c r="F25" t="n">
-        <v>2.4</v>
+        <v>1.5</v>
       </c>
       <c r="G25" t="n">
-        <v>4.8</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="H25" t="n">
-        <v>8.4</v>
+        <v>4.4</v>
       </c>
       <c r="I25" t="n">
-        <v>7.3</v>
+        <v>6.7</v>
       </c>
       <c r="J25" t="n">
-        <v>7.2</v>
+        <v>5.9</v>
       </c>
       <c r="K25" t="n">
-        <v>8.699999999999999</v>
+        <v>3.9</v>
       </c>
       <c r="L25" t="n">
-        <v>5.6</v>
+        <v>3.1</v>
       </c>
     </row>
     <row r="26">
@@ -4507,37 +4507,37 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>9.5</v>
+        <v>7.2</v>
       </c>
       <c r="C26" t="n">
-        <v>9.9</v>
+        <v>6.4</v>
       </c>
       <c r="D26" t="n">
-        <v>5.4</v>
+        <v>4.2</v>
       </c>
       <c r="E26" t="n">
-        <v>2.6</v>
+        <v>5.2</v>
       </c>
       <c r="F26" t="n">
-        <v>3.5</v>
+        <v>7.5</v>
       </c>
       <c r="G26" t="n">
-        <v>6.8</v>
+        <v>7.6</v>
       </c>
       <c r="H26" t="n">
-        <v>4.3</v>
+        <v>2.3</v>
       </c>
       <c r="I26" t="n">
-        <v>5.2</v>
+        <v>5.8</v>
       </c>
       <c r="J26" t="n">
-        <v>6.6</v>
+        <v>5.3</v>
       </c>
       <c r="K26" t="n">
-        <v>6</v>
+        <v>8.1</v>
       </c>
       <c r="L26" t="n">
-        <v>5.6</v>
+        <v>5.1</v>
       </c>
     </row>
     <row r="27">
@@ -4547,37 +4547,37 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>7.2</v>
+        <v>4.4</v>
       </c>
       <c r="C27" t="n">
         <v>9.5</v>
       </c>
       <c r="D27" t="n">
-        <v>7</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E27" t="n">
-        <v>9.6</v>
+        <v>6.8</v>
       </c>
       <c r="F27" t="n">
-        <v>3.6</v>
+        <v>4</v>
       </c>
       <c r="G27" t="n">
-        <v>4.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="H27" t="n">
-        <v>1.2</v>
+        <v>7.2</v>
       </c>
       <c r="I27" t="n">
-        <v>2.9</v>
+        <v>6.4</v>
       </c>
       <c r="J27" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="K27" t="n">
-        <v>4.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="L27" t="n">
-        <v>4.2</v>
+        <v>6.2</v>
       </c>
     </row>
     <row r="28">
@@ -4587,37 +4587,37 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>9</v>
+        <v>6.2</v>
       </c>
       <c r="C28" t="n">
-        <v>5.6</v>
+        <v>6</v>
       </c>
       <c r="D28" t="n">
+        <v>8.199999999999999</v>
+      </c>
+      <c r="E28" t="n">
         <v>4.6</v>
       </c>
-      <c r="E28" t="n">
-        <v>4.8</v>
-      </c>
       <c r="F28" t="n">
-        <v>2.4</v>
+        <v>5.3</v>
       </c>
       <c r="G28" t="n">
-        <v>3.5</v>
+        <v>6.2</v>
       </c>
       <c r="H28" t="n">
-        <v>3.3</v>
+        <v>2.8</v>
       </c>
       <c r="I28" t="n">
-        <v>8</v>
+        <v>7.6</v>
       </c>
       <c r="J28" t="n">
-        <v>9.1</v>
+        <v>7.4</v>
       </c>
       <c r="K28" t="n">
-        <v>7.4</v>
+        <v>6.8</v>
       </c>
       <c r="L28" t="n">
-        <v>9</v>
+        <v>8.6</v>
       </c>
     </row>
     <row r="29">
@@ -4627,37 +4627,37 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>6.2</v>
+        <v>4.3</v>
       </c>
       <c r="C29" t="n">
-        <v>8.6</v>
+        <v>8.5</v>
       </c>
       <c r="D29" t="n">
-        <v>6.2</v>
+        <v>8.199999999999999</v>
       </c>
       <c r="E29" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="F29" t="n">
+        <v>7.4</v>
+      </c>
+      <c r="G29" t="n">
+        <v>7.9</v>
+      </c>
+      <c r="H29" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="I29" t="n">
         <v>3.6</v>
       </c>
-      <c r="F29" t="n">
-        <v>1.9</v>
-      </c>
-      <c r="G29" t="n">
-        <v>4.2</v>
-      </c>
-      <c r="H29" t="n">
-        <v>5.4</v>
-      </c>
-      <c r="I29" t="n">
-        <v>3</v>
-      </c>
       <c r="J29" t="n">
-        <v>7.8</v>
+        <v>4.9</v>
       </c>
       <c r="K29" t="n">
-        <v>3.9</v>
+        <v>5.9</v>
       </c>
       <c r="L29" t="n">
-        <v>5.4</v>
+        <v>3.4</v>
       </c>
     </row>
     <row r="30">
@@ -4667,37 +4667,37 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5.2</v>
+        <v>8.699999999999999</v>
       </c>
       <c r="C30" t="n">
-        <v>7</v>
+        <v>8.9</v>
       </c>
       <c r="D30" t="n">
-        <v>3.7</v>
+        <v>7.4</v>
       </c>
       <c r="E30" t="n">
-        <v>6.2</v>
+        <v>5.4</v>
       </c>
       <c r="F30" t="n">
-        <v>9.9</v>
+        <v>6.5</v>
       </c>
       <c r="G30" t="n">
-        <v>4.4</v>
+        <v>6.8</v>
       </c>
       <c r="H30" t="n">
-        <v>4</v>
+        <v>6.5</v>
       </c>
       <c r="I30" t="n">
-        <v>8</v>
+        <v>8.9</v>
       </c>
       <c r="J30" t="n">
-        <v>7</v>
+        <v>1.8</v>
       </c>
       <c r="K30" t="n">
-        <v>6.5</v>
+        <v>4.1</v>
       </c>
       <c r="L30" t="n">
-        <v>9.1</v>
+        <v>3.8</v>
       </c>
     </row>
     <row r="31">
@@ -4713,31 +4713,31 @@
         <v>9.9</v>
       </c>
       <c r="D31" t="n">
-        <v>5</v>
+        <v>5.6</v>
       </c>
       <c r="E31" t="n">
-        <v>6.9</v>
+        <v>6</v>
       </c>
       <c r="F31" t="n">
-        <v>9.5</v>
+        <v>7.6</v>
       </c>
       <c r="G31" t="n">
         <v>7.7</v>
       </c>
       <c r="H31" t="n">
-        <v>5</v>
+        <v>2.2</v>
       </c>
       <c r="I31" t="n">
-        <v>4.9</v>
+        <v>8.6</v>
       </c>
       <c r="J31" t="n">
         <v>9.300000000000001</v>
       </c>
       <c r="K31" t="n">
-        <v>6.6</v>
+        <v>6.2</v>
       </c>
       <c r="L31" t="n">
-        <v>9.4</v>
+        <v>8.199999999999999</v>
       </c>
     </row>
     <row r="32">
@@ -4747,37 +4747,37 @@
         </is>
       </c>
       <c r="B32" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="C32" t="n">
         <v>8.9</v>
       </c>
-      <c r="C32" t="n">
-        <v>8.6</v>
-      </c>
       <c r="D32" t="n">
-        <v>6.9</v>
+        <v>4.7</v>
       </c>
       <c r="E32" t="n">
-        <v>8.199999999999999</v>
+        <v>6.5</v>
       </c>
       <c r="F32" t="n">
-        <v>6.7</v>
+        <v>8.1</v>
       </c>
       <c r="G32" t="n">
-        <v>4.4</v>
+        <v>6</v>
       </c>
       <c r="H32" t="n">
-        <v>1.1</v>
+        <v>6.4</v>
       </c>
       <c r="I32" t="n">
-        <v>8.199999999999999</v>
+        <v>5.4</v>
       </c>
       <c r="J32" t="n">
-        <v>9.5</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="K32" t="n">
-        <v>5.1</v>
+        <v>7.4</v>
       </c>
       <c r="L32" t="n">
-        <v>5.1</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="33">
@@ -4787,37 +4787,37 @@
         </is>
       </c>
       <c r="B33" t="n">
-        <v>3.2</v>
+        <v>8.5</v>
       </c>
       <c r="C33" t="n">
-        <v>8.6</v>
+        <v>9.199999999999999</v>
       </c>
       <c r="D33" t="n">
-        <v>7.9</v>
+        <v>6</v>
       </c>
       <c r="E33" t="n">
-        <v>3.9</v>
+        <v>7.2</v>
       </c>
       <c r="F33" t="n">
-        <v>3.2</v>
+        <v>10</v>
       </c>
       <c r="G33" t="n">
+        <v>8.800000000000001</v>
+      </c>
+      <c r="H33" t="n">
         <v>5.6</v>
       </c>
-      <c r="H33" t="n">
-        <v>7.6</v>
-      </c>
       <c r="I33" t="n">
-        <v>7.2</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="J33" t="n">
-        <v>5.5</v>
+        <v>4.6</v>
       </c>
       <c r="K33" t="n">
-        <v>8.800000000000001</v>
+        <v>7</v>
       </c>
       <c r="L33" t="n">
-        <v>9.6</v>
+        <v>4.9</v>
       </c>
     </row>
     <row r="34">
@@ -4827,37 +4827,37 @@
         </is>
       </c>
       <c r="B34" t="n">
-        <v>8.699999999999999</v>
+        <v>8.9</v>
       </c>
       <c r="C34" t="n">
-        <v>7.1</v>
+        <v>3.7</v>
       </c>
       <c r="D34" t="n">
-        <v>4.6</v>
+        <v>7</v>
       </c>
       <c r="E34" t="n">
-        <v>4.7</v>
+        <v>8.4</v>
       </c>
       <c r="F34" t="n">
-        <v>5.4</v>
+        <v>9.300000000000001</v>
       </c>
       <c r="G34" t="n">
-        <v>3</v>
+        <v>4.2</v>
       </c>
       <c r="H34" t="n">
-        <v>3</v>
+        <v>8.6</v>
       </c>
       <c r="I34" t="n">
-        <v>0.6</v>
+        <v>7.4</v>
       </c>
       <c r="J34" t="n">
-        <v>8.9</v>
+        <v>8</v>
       </c>
       <c r="K34" t="n">
-        <v>9.699999999999999</v>
+        <v>8.4</v>
       </c>
       <c r="L34" t="n">
-        <v>1.3</v>
+        <v>4.2</v>
       </c>
     </row>
     <row r="35">
@@ -4867,34 +4867,34 @@
         </is>
       </c>
       <c r="B35" t="n">
-        <v>9.6</v>
+        <v>7.6</v>
       </c>
       <c r="C35" t="n">
-        <v>7.1</v>
+        <v>9</v>
       </c>
       <c r="D35" t="n">
-        <v>4.4</v>
+        <v>7.4</v>
       </c>
       <c r="E35" t="n">
-        <v>4.3</v>
+        <v>3.2</v>
       </c>
       <c r="F35" t="n">
-        <v>5.5</v>
+        <v>1</v>
       </c>
       <c r="G35" t="n">
-        <v>1.1</v>
+        <v>5</v>
       </c>
       <c r="H35" t="n">
-        <v>5.6</v>
+        <v>7.2</v>
       </c>
       <c r="I35" t="n">
-        <v>5</v>
+        <v>4.8</v>
       </c>
       <c r="J35" t="n">
         <v>9</v>
       </c>
       <c r="K35" t="n">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="L35" t="n">
         <v>3.4</v>
@@ -4907,37 +4907,37 @@
         </is>
       </c>
       <c r="B36" t="n">
-        <v>6.6</v>
+        <v>7.6</v>
       </c>
       <c r="C36" t="n">
         <v>8.300000000000001</v>
       </c>
       <c r="D36" t="n">
-        <v>8.4</v>
+        <v>8.800000000000001</v>
       </c>
       <c r="E36" t="n">
-        <v>7.5</v>
+        <v>3.4</v>
       </c>
       <c r="F36" t="n">
-        <v>3.4</v>
+        <v>8</v>
       </c>
       <c r="G36" t="n">
-        <v>8.300000000000001</v>
+        <v>9.699999999999999</v>
       </c>
       <c r="H36" t="n">
-        <v>7.4</v>
+        <v>7</v>
       </c>
       <c r="I36" t="n">
-        <v>8.699999999999999</v>
+        <v>10</v>
       </c>
       <c r="J36" t="n">
-        <v>9</v>
+        <v>9.6</v>
       </c>
       <c r="K36" t="n">
-        <v>8.199999999999999</v>
+        <v>4.3</v>
       </c>
       <c r="L36" t="n">
-        <v>4.9</v>
+        <v>5.4</v>
       </c>
     </row>
     <row r="37">
@@ -4947,37 +4947,37 @@
         </is>
       </c>
       <c r="B37" t="n">
-        <v>7.5</v>
+        <v>4.3</v>
       </c>
       <c r="C37" t="n">
-        <v>6.2</v>
+        <v>9</v>
       </c>
       <c r="D37" t="n">
-        <v>5.9</v>
+        <v>4.7</v>
       </c>
       <c r="E37" t="n">
-        <v>6.1</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="F37" t="n">
-        <v>1.9</v>
+        <v>4.1</v>
       </c>
       <c r="G37" t="n">
-        <v>3.4</v>
+        <v>5.8</v>
       </c>
       <c r="H37" t="n">
-        <v>1.1</v>
+        <v>1.5</v>
       </c>
       <c r="I37" t="n">
-        <v>8.4</v>
+        <v>2.6</v>
       </c>
       <c r="J37" t="n">
-        <v>9.699999999999999</v>
+        <v>7.1</v>
       </c>
       <c r="K37" t="n">
-        <v>4.2</v>
+        <v>8.6</v>
       </c>
       <c r="L37" t="n">
-        <v>2.4</v>
+        <v>2.9</v>
       </c>
     </row>
   </sheetData>
@@ -5000,6 +5000,11 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Trimestres</t>
+        </is>
+      </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
           <t>FIL</t>
@@ -5143,37 +5148,37 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>7.53888888888889</v>
+        <v>7.144444444444444</v>
       </c>
       <c r="C4" t="n">
-        <v>7.872222222222224</v>
+        <v>7.613888888888888</v>
       </c>
       <c r="D4" t="n">
-        <v>6.272222222222222</v>
+        <v>6.941666666666666</v>
       </c>
       <c r="E4" t="n">
-        <v>6.544444444444444</v>
+        <v>6.677777777777778</v>
       </c>
       <c r="F4" t="n">
-        <v>5.811111111111112</v>
+        <v>6.213888888888889</v>
       </c>
       <c r="G4" t="n">
-        <v>6.372222222222224</v>
+        <v>6.994444444444444</v>
       </c>
       <c r="H4" t="n">
-        <v>4.336111111111111</v>
+        <v>4.469444444444444</v>
       </c>
       <c r="I4" t="n">
-        <v>6.591666666666666</v>
+        <v>6.913888888888889</v>
       </c>
       <c r="J4" t="n">
-        <v>7.183333333333334</v>
+        <v>6.913888888888888</v>
       </c>
       <c r="K4" t="n">
-        <v>6.252777777777776</v>
+        <v>6.938888888888889</v>
       </c>
       <c r="L4" t="n">
-        <v>6.661111111111112</v>
+        <v>6.300000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>